<commit_message>
EPBDS-9540 Support Java Name convestion on Json field name generating in SpreadsheetResults
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8844_Collections_of_SRs.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8844_Collections_of_SRs.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkama\.openl\user-workspace\DEFAULT\EPBDS-8844_Collections_of_SRs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BDC02C-F34F-4D0A-9B8A-54F19C986F4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="27795" windowHeight="10290"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="194">
   <si>
     <t>Datatype MyType</t>
   </si>
@@ -408,39 +414,12 @@
     <t>=(Map)$Step3[1][1]</t>
   </si>
   <si>
-    <t>_res_.$Step4["Step1"]</t>
-  </si>
-  <si>
-    <t>_res_.$Step4["Step1"]:Integer</t>
-  </si>
-  <si>
-    <t>_res_.$Step5["Step1"]:Integer</t>
-  </si>
-  <si>
-    <t>_res_.$Step6["Step1"]:Integer</t>
-  </si>
-  <si>
-    <t>_res_.$Step7["Step1"]:Integer</t>
-  </si>
-  <si>
     <t>Step10</t>
   </si>
   <si>
     <t>Step11</t>
   </si>
   <si>
-    <t>=((MyType)((Map)$Step3[0][0])["Step7"]).someText</t>
-  </si>
-  <si>
-    <t>=((MyType)((Map)$Step3[0][1])["Step7"]).someText</t>
-  </si>
-  <si>
-    <t>=((MyType)((Map)$Step3[1][0])["Step7"]).someText</t>
-  </si>
-  <si>
-    <t>=((MyType)((Map)$Step3[1][1])["Step7"]).someText</t>
-  </si>
-  <si>
     <t>_res_.$Step8</t>
   </si>
   <si>
@@ -471,18 +450,6 @@
     <t>=((Map[])$Step3[1])[1]</t>
   </si>
   <si>
-    <t>=((MyType)(((Map[])$Step3[0])[0])["Step7"]).someText</t>
-  </si>
-  <si>
-    <t>=((MyType)(((Map[])$Step3[0])[1])["Step7"]).someText</t>
-  </si>
-  <si>
-    <t>=((MyType)(((Map[])$Step3[1])[0])["Step7"]).someText</t>
-  </si>
-  <si>
-    <t>=((MyType)(((Map[])$Step3[1])[1])["Step7"]).someText</t>
-  </si>
-  <si>
     <t>List [] []</t>
   </si>
   <si>
@@ -510,9 +477,6 @@
     <t>Spreadsheet SpreadsheetResult   simplSp_List_of_List_toMap(Integer a, String b, List f)</t>
   </si>
   <si>
-    <t>_res_.$Step3["Step1"]</t>
-  </si>
-  <si>
     <t>=(Map)((List)(((Map)$Step2[0])["Calc"]))[0]</t>
   </si>
   <si>
@@ -525,18 +489,6 @@
     <t>=(Map)((List)(((Map)$Step2[1])["Calc"]))[1]</t>
   </si>
   <si>
-    <t>_res_.$Step5["Step1"]</t>
-  </si>
-  <si>
-    <t>_res_.$Step6["Step1"]</t>
-  </si>
-  <si>
-    <t>_res_.$Step3["Step1"]:Integer</t>
-  </si>
-  <si>
-    <t>=((MyType)(((Map)((List)(((Map)$Step2[1])["Calc"]))[1])["Step7"])).someMap</t>
-  </si>
-  <si>
     <t>_res_.$Step7["someKey"]</t>
   </si>
   <si>
@@ -556,16 +508,113 @@
   </si>
   <si>
     <t>Map of Srs</t>
+  </si>
+  <si>
+    <t>_res_.$Step4["step1"]:Integer</t>
+  </si>
+  <si>
+    <t>_res_.$Step5["step1"]:Integer</t>
+  </si>
+  <si>
+    <t>_res_.$Step6["step1"]:Integer</t>
+  </si>
+  <si>
+    <t>_res_.$Step7["step1"]:Integer</t>
+  </si>
+  <si>
+    <t>=((MyType)((Map)$Step3[0][0])["step7"]).someText</t>
+  </si>
+  <si>
+    <t>=((MyType)((Map)$Step3[0][1])["step7"]).someText</t>
+  </si>
+  <si>
+    <t>=((MyType)((Map)$Step3[1][0])["step7"]).someText</t>
+  </si>
+  <si>
+    <t>=((MyType)((Map)$Step3[1][1])["step7"]).someText</t>
+  </si>
+  <si>
+    <t>=((MyType)(((Map[])$Step3[0])[0])["step7"]).someText</t>
+  </si>
+  <si>
+    <t>=((MyType)(((Map[])$Step3[0])[1])["step7"]).someText</t>
+  </si>
+  <si>
+    <t>=((MyType)(((Map[])$Step3[1])[0])["step7"]).someText</t>
+  </si>
+  <si>
+    <t>=((MyType)(((Map[])$Step3[1])[1])["step7"]).someText</t>
+  </si>
+  <si>
+    <t>=((MyType)(((Map)((List)(((Map)$Step2[1])["Calc"]))[1])["step7"])).someMap</t>
+  </si>
+  <si>
+    <t>_res_.$Step3["step1"]:Integer</t>
+  </si>
+  <si>
+    <t>_res_.$Step3["step1"]</t>
+  </si>
+  <si>
+    <t>_res_.$Step4["step1"]</t>
+  </si>
+  <si>
+    <t>_res_.$Step5["step1"]</t>
+  </si>
+  <si>
+    <t>_res_.$Step6["step1"]</t>
+  </si>
+  <si>
+    <t>=(Map[][])$Step2["calc"]</t>
+  </si>
+  <si>
+    <t>=(List)$Step2["calc"]</t>
+  </si>
+  <si>
+    <t>=((Map)$Step3[0])["step1"]</t>
+  </si>
+  <si>
+    <t>=((Map)$Step3[1])["step1"]</t>
+  </si>
+  <si>
+    <t>=(Map)((List)(((Map)$Step2[0])["calc"]))[0]</t>
+  </si>
+  <si>
+    <t>=(Map)((List)(((Map)$Step2[0])["calc"]))[1]</t>
+  </si>
+  <si>
+    <t>=(Map)((List)(((Map)$Step2[1])["calc"]))[0]</t>
+  </si>
+  <si>
+    <t>=(Map)((List)(((Map)$Step2[1])["calc"]))[1]</t>
+  </si>
+  <si>
+    <t>=((MyType)(((Map)((List)(((Map)$Step2[1])["calc"]))[1])["step7"])).someMap</t>
+  </si>
+  <si>
+    <t>=(List)$Step1.toMap()["calc"]</t>
+  </si>
+  <si>
+    <t>=$Step2["calc"]</t>
+  </si>
+  <si>
+    <t>=((Passport)((MyType)((Map)$Step4)["step7"]).passportData).passportId</t>
+  </si>
+  <si>
+    <t>=((MyType)((Map)$Step4)["step7"]).someMap</t>
+  </si>
+  <si>
+    <t>=(List)((MyType)((Map)$Step4)["step7"]).someList</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="1" rgb="000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -600,13 +649,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="0" tint="-0.14999847407452621" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
+        <fgColor theme="6" tint="0.59999389629810485" rgb="9BBB59"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -618,7 +667,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
+        <fgColor theme="6" tint="0.79998168889431442" rgb="9BBB59"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -715,9 +764,9 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0" xfId="2"/>
   </cellStyleXfs>
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -736,6 +785,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -748,9 +801,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -760,12 +810,11 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="2" builtinId="24"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Вычисление" xfId="1" builtinId="22"/>
+    <cellStyle name="Связанная ячейка" xfId="2" builtinId="24"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -792,7 +841,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -801,14 +850,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -846,9 +898,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -881,9 +933,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -916,9 +985,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1091,45 +1177,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:S104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="21" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="51.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="61.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="29" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="51.59765625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="61.59765625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="24.73046875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.3984375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.3984375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="21.86328125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B1" s="7" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="2" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B4" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="E4" s="16" t="s">
+      <c r="C4" s="18"/>
+      <c r="E4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="16"/>
+      <c r="F4" s="18"/>
       <c r="H4" s="8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1146,7 +1232,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1163,7 +1249,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
@@ -1177,7 +1263,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
@@ -1185,7 +1271,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
@@ -1193,7 +1279,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
@@ -1201,7 +1287,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B11" s="2" t="s">
         <v>76</v>
       </c>
@@ -1209,13 +1295,13 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="14" t="s">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B15" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="15"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="17"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B16" s="11" t="s">
         <v>21</v>
       </c>
@@ -1223,7 +1309,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B17" s="12" t="s">
         <v>32</v>
       </c>
@@ -1231,7 +1317,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B18" s="11" t="s">
         <v>42</v>
       </c>
@@ -1239,7 +1325,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B19" s="11" t="s">
         <v>78</v>
       </c>
@@ -1247,7 +1333,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B20" s="11" t="s">
         <v>81</v>
       </c>
@@ -1255,7 +1341,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B21" s="11" t="s">
         <v>43</v>
       </c>
@@ -1263,7 +1349,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B22" s="11" t="s">
         <v>44</v>
       </c>
@@ -1271,7 +1357,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="2:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B23" s="12" t="s">
         <v>39</v>
       </c>
@@ -1279,7 +1365,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="2:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B24" s="11" t="s">
         <v>45</v>
       </c>
@@ -1287,7 +1373,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B25" s="12" t="s">
         <v>38</v>
       </c>
@@ -1295,15 +1381,15 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B28" s="14" t="s">
+    <row r="28" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="B28" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="15"/>
+      <c r="C28" s="17"/>
       <c r="I28" s="2"/>
       <c r="S28" s="2"/>
     </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B29" s="11" t="s">
         <v>21</v>
       </c>
@@ -1311,7 +1397,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B30" s="11" t="s">
         <v>41</v>
       </c>
@@ -1320,34 +1406,34 @@
       </c>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:19" x14ac:dyDescent="0.45">
       <c r="C31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:19" x14ac:dyDescent="0.45">
       <c r="C32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="22" t="s">
-        <v>178</v>
+    <row r="33" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B33" s="14" t="s">
+        <v>160</v>
       </c>
       <c r="C33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="C34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B35" s="14" t="s">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B35" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="15"/>
+      <c r="C35" s="17"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B36" s="11" t="s">
         <v>21</v>
       </c>
@@ -1356,7 +1442,7 @@
       </c>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B37" s="11" t="s">
         <v>53</v>
       </c>
@@ -1366,7 +1452,7 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B38" s="11" t="s">
         <v>42</v>
       </c>
@@ -1376,7 +1462,7 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B39" s="11" t="s">
         <v>58</v>
       </c>
@@ -1386,7 +1472,7 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B40" s="11" t="s">
         <v>44</v>
       </c>
@@ -1396,7 +1482,7 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B41" s="11" t="s">
         <v>69</v>
       </c>
@@ -1406,7 +1492,7 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B42" s="11" t="s">
         <v>45</v>
       </c>
@@ -1416,7 +1502,7 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B43" s="11" t="s">
         <v>72</v>
       </c>
@@ -1426,7 +1512,7 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B44" s="11" t="s">
         <v>75</v>
       </c>
@@ -1436,7 +1522,7 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B45" s="11" t="s">
         <v>83</v>
       </c>
@@ -1446,34 +1532,34 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B46" s="11" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.45">
       <c r="I47" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B48" s="14" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B48" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="C48" s="17"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="17"/>
-      <c r="G48" s="17"/>
-      <c r="H48" s="17"/>
-      <c r="I48" s="15"/>
-    </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C48" s="19"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="19"/>
+      <c r="I48" s="17"/>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B49" s="11" t="s">
         <v>34</v>
       </c>
@@ -1496,10 +1582,10 @@
         <v>89</v>
       </c>
       <c r="I49" s="11" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B50" s="11" t="s">
         <v>34</v>
       </c>
@@ -1522,10 +1608,10 @@
         <v>89</v>
       </c>
       <c r="I50" s="11" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B51" s="2" t="s">
         <v>36</v>
       </c>
@@ -1549,13 +1635,13 @@
       </c>
       <c r="I51" s="2"/>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B54" s="18" t="s">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B54" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C54" s="18"/>
-    </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C54" s="15"/>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B55" s="11" t="s">
         <v>21</v>
       </c>
@@ -1563,7 +1649,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B56" s="11" t="s">
         <v>40</v>
       </c>
@@ -1571,7 +1657,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B57" s="11" t="s">
         <v>46</v>
       </c>
@@ -1579,7 +1665,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B58" s="12" t="s">
         <v>63</v>
       </c>
@@ -1587,14 +1673,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B61" s="18" t="s">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B61" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C61" s="18"/>
+      <c r="C61" s="15"/>
       <c r="H61" s="1"/>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B62" s="11" t="s">
         <v>21</v>
       </c>
@@ -1602,7 +1688,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B63" s="11" t="s">
         <v>53</v>
       </c>
@@ -1611,7 +1697,7 @@
       </c>
       <c r="H63" s="1"/>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B64" s="11" t="s">
         <v>42</v>
       </c>
@@ -1620,46 +1706,46 @@
       </c>
       <c r="H64" s="1"/>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B65" s="11" t="s">
         <v>58</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>67</v>
+        <v>181</v>
       </c>
       <c r="H65" s="1"/>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B66" s="11" t="s">
         <v>44</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B67" s="11" t="s">
         <v>69</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C68" s="1"/>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C69" s="1"/>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B71" s="18" t="s">
+    <row r="71" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B71" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="C71" s="18"/>
-      <c r="D71" s="18"/>
-      <c r="E71" s="18"/>
-    </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C71" s="15"/>
+      <c r="D71" s="15"/>
+      <c r="E71" s="15"/>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B72" s="11" t="s">
         <v>34</v>
       </c>
@@ -1673,7 +1759,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B73" s="11" t="s">
         <v>34</v>
       </c>
@@ -1687,7 +1773,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B74" s="2">
         <v>1</v>
       </c>
@@ -1701,19 +1787,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="22" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="77" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B78" s="18" t="s">
+    <row r="76" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B76" s="14" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B78" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="C78" s="18"/>
-    </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C78" s="15"/>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B79" s="11" t="s">
         <v>21</v>
       </c>
@@ -1721,7 +1807,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B80" s="12" t="s">
         <v>102</v>
       </c>
@@ -1729,7 +1815,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B81" s="12" t="s">
         <v>103</v>
       </c>
@@ -1737,7 +1823,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B82" s="12" t="s">
         <v>104</v>
       </c>
@@ -1745,7 +1831,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B83" s="12" t="s">
         <v>105</v>
       </c>
@@ -1753,7 +1839,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B84" s="12" t="s">
         <v>106</v>
       </c>
@@ -1761,7 +1847,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B85" s="12" t="s">
         <v>63</v>
       </c>
@@ -1769,14 +1855,14 @@
         <v>52</v>
       </c>
     </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B89" s="18" t="s">
+    <row r="89" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B89" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="C89" s="18"/>
+      <c r="C89" s="15"/>
       <c r="G89" s="1"/>
     </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B90" s="11" t="s">
         <v>21</v>
       </c>
@@ -1784,7 +1870,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B91" s="11" t="s">
         <v>53</v>
       </c>
@@ -1793,7 +1879,7 @@
       </c>
       <c r="G91" s="1"/>
     </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B92" s="11" t="s">
         <v>42</v>
       </c>
@@ -1802,16 +1888,16 @@
       </c>
       <c r="G92" s="1"/>
     </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B93" s="11" t="s">
         <v>58</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>107</v>
+        <v>190</v>
       </c>
       <c r="G93" s="1"/>
     </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B94" s="11" t="s">
         <v>44</v>
       </c>
@@ -1819,40 +1905,40 @@
         <v>109</v>
       </c>
     </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B95" s="11" t="s">
         <v>45</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B96" s="11" t="s">
         <v>75</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="97" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B97" s="11" t="s">
         <v>83</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B101" s="18" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B101" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="C101" s="18"/>
-      <c r="D101" s="18"/>
-      <c r="E101" s="18"/>
-      <c r="F101" s="18"/>
-    </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C101" s="15"/>
+      <c r="D101" s="15"/>
+      <c r="E101" s="15"/>
+      <c r="F101" s="15"/>
+    </row>
+    <row r="102" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B102" s="11" t="s">
         <v>34</v>
       </c>
@@ -1869,7 +1955,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B103" s="11" t="s">
         <v>34</v>
       </c>
@@ -1886,7 +1972,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B104" s="2">
         <v>1</v>
       </c>
@@ -1905,59 +1991,59 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B48:I48"/>
+    <mergeCell ref="B15:C15"/>
     <mergeCell ref="B54:C54"/>
     <mergeCell ref="B101:F101"/>
     <mergeCell ref="B89:C89"/>
     <mergeCell ref="B78:C78"/>
     <mergeCell ref="B71:E71"/>
     <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="B48:I48"/>
-    <mergeCell ref="B15:C15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M85"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="52.42578125" customWidth="1"/>
-    <col min="4" max="4" width="29.5703125" customWidth="1"/>
-    <col min="5" max="5" width="23" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" customWidth="1"/>
-    <col min="7" max="7" width="33" customWidth="1"/>
-    <col min="8" max="8" width="28.140625" customWidth="1"/>
-    <col min="9" max="9" width="29" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="22.1328125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="52.3984375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="29.59765625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.3984375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="28.1328125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.59765625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="12.86328125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" s="6"/>
       <c r="B1" s="5" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="C1" s="6"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="20" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="B3" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="C3" s="21"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C3" s="22"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B4" s="11" t="s">
         <v>21</v>
       </c>
@@ -1965,7 +2051,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B5" s="11" t="s">
         <v>40</v>
       </c>
@@ -1973,7 +2059,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B6" s="11" t="s">
         <v>46</v>
       </c>
@@ -1981,7 +2067,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B7" s="12" t="s">
         <v>99</v>
       </c>
@@ -1989,17 +2075,17 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="19" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="B9" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="C9" s="19"/>
+      <c r="C9" s="20"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B10" s="11" t="s">
         <v>21</v>
       </c>
@@ -2007,7 +2093,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B11" s="11" t="s">
         <v>53</v>
       </c>
@@ -2016,7 +2102,7 @@
       </c>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B12" s="11" t="s">
         <v>42</v>
       </c>
@@ -2025,16 +2111,16 @@
       </c>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B13" s="11" t="s">
         <v>58</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>114</v>
+        <v>180</v>
       </c>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B14" s="11" t="s">
         <v>44</v>
       </c>
@@ -2043,7 +2129,7 @@
       </c>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B15" s="11" t="s">
         <v>69</v>
       </c>
@@ -2052,7 +2138,7 @@
       </c>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B16" s="11" t="s">
         <v>45</v>
       </c>
@@ -2061,7 +2147,7 @@
       </c>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B17" s="11" t="s">
         <v>72</v>
       </c>
@@ -2070,64 +2156,64 @@
       </c>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B18" s="11" t="s">
         <v>75</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B19" s="11" t="s">
         <v>83</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B20" s="11" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B21" s="11" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.45">
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.45">
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.45">
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="19" t="s">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B25" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19"/>
-      <c r="M25" s="19"/>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="20"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B26" s="11" t="s">
         <v>120</v>
       </c>
@@ -2141,31 +2227,31 @@
         <v>123</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>131</v>
+        <v>162</v>
       </c>
       <c r="G26" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="I26" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="J26" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="H26" s="11" t="s">
+      <c r="K26" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="I26" s="11" t="s">
+      <c r="L26" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="J26" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="K26" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="L26" s="11" t="s">
-        <v>143</v>
-      </c>
       <c r="M26" s="11" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B27" s="11" t="s">
         <v>120</v>
       </c>
@@ -2179,31 +2265,31 @@
         <v>123</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>131</v>
+        <v>162</v>
       </c>
       <c r="G27" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="J27" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="H27" s="11" t="s">
+      <c r="K27" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="I27" s="11" t="s">
+      <c r="L27" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="J27" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="K27" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="L27" s="11" t="s">
-        <v>143</v>
-      </c>
       <c r="M27" s="11" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B28" s="2">
         <v>1</v>
       </c>
@@ -2241,22 +2327,22 @@
         <v>125</v>
       </c>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.45">
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.45">
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.45">
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="19" t="s">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B32" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="C32" s="19"/>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C32" s="20"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B33" s="11" t="s">
         <v>21</v>
       </c>
@@ -2264,7 +2350,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B34" s="11" t="s">
         <v>40</v>
       </c>
@@ -2272,7 +2358,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B35" s="11" t="s">
         <v>46</v>
       </c>
@@ -2280,7 +2366,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B36" s="12" t="s">
         <v>99</v>
       </c>
@@ -2288,18 +2374,18 @@
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B39" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41" s="19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B41" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="C41" s="19"/>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C41" s="20"/>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B42" s="11" t="s">
         <v>21</v>
       </c>
@@ -2307,7 +2393,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B43" s="11" t="s">
         <v>53</v>
       </c>
@@ -2315,7 +2401,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B44" s="11" t="s">
         <v>42</v>
       </c>
@@ -2323,101 +2409,101 @@
         <v>64</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B45" s="11" t="s">
         <v>58</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B46" s="11" t="s">
         <v>44</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B47" s="11" t="s">
         <v>69</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B48" s="11" t="s">
         <v>45</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B49" s="11" t="s">
         <v>72</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B50" s="11" t="s">
         <v>75</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B51" s="11" t="s">
         <v>83</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B52" s="11" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B53" s="11" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.45">
       <c r="C54" s="1"/>
     </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:13" x14ac:dyDescent="0.45">
       <c r="C55" s="1"/>
     </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B57" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="C57" s="19"/>
-      <c r="D57" s="19"/>
-      <c r="E57" s="19"/>
-      <c r="F57" s="19"/>
-      <c r="G57" s="19"/>
-      <c r="H57" s="19"/>
-      <c r="I57" s="19"/>
-      <c r="J57" s="19"/>
-      <c r="K57" s="19"/>
-      <c r="L57" s="19"/>
-      <c r="M57" s="19"/>
-    </row>
-    <row r="58" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B57" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="C57" s="20"/>
+      <c r="D57" s="20"/>
+      <c r="E57" s="20"/>
+      <c r="F57" s="20"/>
+      <c r="G57" s="20"/>
+      <c r="H57" s="20"/>
+      <c r="I57" s="20"/>
+      <c r="J57" s="20"/>
+      <c r="K57" s="20"/>
+      <c r="L57" s="20"/>
+      <c r="M57" s="20"/>
+    </row>
+    <row r="58" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B58" s="11" t="s">
         <v>120</v>
       </c>
@@ -2431,31 +2517,31 @@
         <v>123</v>
       </c>
       <c r="F58" s="11" t="s">
-        <v>131</v>
+        <v>162</v>
       </c>
       <c r="G58" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="H58" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="I58" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="J58" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="H58" s="11" t="s">
+      <c r="K58" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="I58" s="11" t="s">
+      <c r="L58" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="J58" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="K58" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="L58" s="11" t="s">
-        <v>143</v>
-      </c>
       <c r="M58" s="11" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="59" spans="2:13" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="59" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B59" s="11" t="s">
         <v>120</v>
       </c>
@@ -2469,31 +2555,31 @@
         <v>123</v>
       </c>
       <c r="F59" s="11" t="s">
-        <v>131</v>
+        <v>162</v>
       </c>
       <c r="G59" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="H59" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="I59" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="J59" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="H59" s="11" t="s">
+      <c r="K59" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="I59" s="11" t="s">
+      <c r="L59" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="J59" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="K59" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="L59" s="11" t="s">
-        <v>143</v>
-      </c>
       <c r="M59" s="11" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="60" spans="2:13" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="60" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B60" s="2">
         <v>1</v>
       </c>
@@ -2531,19 +2617,19 @@
         <v>125</v>
       </c>
     </row>
-    <row r="63" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B63" s="7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="64" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B66" s="19" t="s">
-        <v>158</v>
-      </c>
-      <c r="C66" s="19"/>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="64" spans="2:13" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B66" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="C66" s="20"/>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B67" s="11" t="s">
         <v>21</v>
       </c>
@@ -2551,23 +2637,23 @@
         <v>33</v>
       </c>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B68" s="11" t="s">
         <v>40</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B69" s="11" t="s">
         <v>46</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B70" s="11" t="s">
         <v>99</v>
       </c>
@@ -2576,13 +2662,13 @@
       </c>
       <c r="D70" s="1"/>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B72" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="C72" s="19"/>
-    </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B72" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="C72" s="20"/>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B73" s="11" t="s">
         <v>21</v>
       </c>
@@ -2590,120 +2676,120 @@
         <v>22</v>
       </c>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B74" s="11" t="s">
         <v>53</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B75" s="11" t="s">
         <v>42</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B76" s="11" t="s">
         <v>58</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B77" s="11" t="s">
         <v>44</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B78" s="11" t="s">
         <v>69</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B79" s="11" t="s">
         <v>45</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B80" s="11" t="s">
         <v>72</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B82" s="19" t="s">
-        <v>160</v>
-      </c>
-      <c r="C82" s="19"/>
-      <c r="D82" s="19"/>
-      <c r="E82" s="19"/>
-      <c r="F82" s="19"/>
-      <c r="G82" s="19"/>
-      <c r="H82" s="19"/>
-    </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B82" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="C82" s="20"/>
+      <c r="D82" s="20"/>
+      <c r="E82" s="20"/>
+      <c r="F82" s="20"/>
+      <c r="G82" s="20"/>
+      <c r="H82" s="20"/>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B83" s="11" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="C83" s="11" t="s">
         <v>35</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="E83" s="11" t="s">
-        <v>131</v>
+        <v>162</v>
       </c>
       <c r="F83" s="11" t="s">
-        <v>132</v>
+        <v>163</v>
       </c>
       <c r="G83" s="11" t="s">
-        <v>133</v>
+        <v>164</v>
       </c>
       <c r="H83" s="11" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B84" s="11" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="C84" s="11" t="s">
         <v>35</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="E84" s="11" t="s">
-        <v>130</v>
+        <v>177</v>
       </c>
       <c r="F84" s="11" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="G84" s="11" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="H84" s="11" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B85" s="2">
         <v>1</v>
       </c>
@@ -2743,12 +2829,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
EPBDS-9540 Support Java Name convestion on Json field name generating in SpreadsheetResults. Rework.
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8844_Collections_of_SRs.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8844_Collections_of_SRs.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkama\.openl\user-workspace\DEFAULT\EPBDS-8844_Collections_of_SRs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BDC02C-F34F-4D0A-9B8A-54F19C986F4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="27795" windowHeight="10290"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="180">
   <si>
     <t>Datatype MyType</t>
   </si>
@@ -414,12 +408,39 @@
     <t>=(Map)$Step3[1][1]</t>
   </si>
   <si>
+    <t>_res_.$Step4["Step1"]</t>
+  </si>
+  <si>
+    <t>_res_.$Step4["Step1"]:Integer</t>
+  </si>
+  <si>
+    <t>_res_.$Step5["Step1"]:Integer</t>
+  </si>
+  <si>
+    <t>_res_.$Step6["Step1"]:Integer</t>
+  </si>
+  <si>
+    <t>_res_.$Step7["Step1"]:Integer</t>
+  </si>
+  <si>
     <t>Step10</t>
   </si>
   <si>
     <t>Step11</t>
   </si>
   <si>
+    <t>=((MyType)((Map)$Step3[0][0])["Step7"]).someText</t>
+  </si>
+  <si>
+    <t>=((MyType)((Map)$Step3[0][1])["Step7"]).someText</t>
+  </si>
+  <si>
+    <t>=((MyType)((Map)$Step3[1][0])["Step7"]).someText</t>
+  </si>
+  <si>
+    <t>=((MyType)((Map)$Step3[1][1])["Step7"]).someText</t>
+  </si>
+  <si>
     <t>_res_.$Step8</t>
   </si>
   <si>
@@ -450,6 +471,18 @@
     <t>=((Map[])$Step3[1])[1]</t>
   </si>
   <si>
+    <t>=((MyType)(((Map[])$Step3[0])[0])["Step7"]).someText</t>
+  </si>
+  <si>
+    <t>=((MyType)(((Map[])$Step3[0])[1])["Step7"]).someText</t>
+  </si>
+  <si>
+    <t>=((MyType)(((Map[])$Step3[1])[0])["Step7"]).someText</t>
+  </si>
+  <si>
+    <t>=((MyType)(((Map[])$Step3[1])[1])["Step7"]).someText</t>
+  </si>
+  <si>
     <t>List [] []</t>
   </si>
   <si>
@@ -477,6 +510,9 @@
     <t>Spreadsheet SpreadsheetResult   simplSp_List_of_List_toMap(Integer a, String b, List f)</t>
   </si>
   <si>
+    <t>_res_.$Step3["Step1"]</t>
+  </si>
+  <si>
     <t>=(Map)((List)(((Map)$Step2[0])["Calc"]))[0]</t>
   </si>
   <si>
@@ -489,6 +525,18 @@
     <t>=(Map)((List)(((Map)$Step2[1])["Calc"]))[1]</t>
   </si>
   <si>
+    <t>_res_.$Step5["Step1"]</t>
+  </si>
+  <si>
+    <t>_res_.$Step6["Step1"]</t>
+  </si>
+  <si>
+    <t>_res_.$Step3["Step1"]:Integer</t>
+  </si>
+  <si>
+    <t>=((MyType)(((Map)((List)(((Map)$Step2[1])["Calc"]))[1])["Step7"])).someMap</t>
+  </si>
+  <si>
     <t>_res_.$Step7["someKey"]</t>
   </si>
   <si>
@@ -508,113 +556,16 @@
   </si>
   <si>
     <t>Map of Srs</t>
-  </si>
-  <si>
-    <t>_res_.$Step4["step1"]:Integer</t>
-  </si>
-  <si>
-    <t>_res_.$Step5["step1"]:Integer</t>
-  </si>
-  <si>
-    <t>_res_.$Step6["step1"]:Integer</t>
-  </si>
-  <si>
-    <t>_res_.$Step7["step1"]:Integer</t>
-  </si>
-  <si>
-    <t>=((MyType)((Map)$Step3[0][0])["step7"]).someText</t>
-  </si>
-  <si>
-    <t>=((MyType)((Map)$Step3[0][1])["step7"]).someText</t>
-  </si>
-  <si>
-    <t>=((MyType)((Map)$Step3[1][0])["step7"]).someText</t>
-  </si>
-  <si>
-    <t>=((MyType)((Map)$Step3[1][1])["step7"]).someText</t>
-  </si>
-  <si>
-    <t>=((MyType)(((Map[])$Step3[0])[0])["step7"]).someText</t>
-  </si>
-  <si>
-    <t>=((MyType)(((Map[])$Step3[0])[1])["step7"]).someText</t>
-  </si>
-  <si>
-    <t>=((MyType)(((Map[])$Step3[1])[0])["step7"]).someText</t>
-  </si>
-  <si>
-    <t>=((MyType)(((Map[])$Step3[1])[1])["step7"]).someText</t>
-  </si>
-  <si>
-    <t>=((MyType)(((Map)((List)(((Map)$Step2[1])["Calc"]))[1])["step7"])).someMap</t>
-  </si>
-  <si>
-    <t>_res_.$Step3["step1"]:Integer</t>
-  </si>
-  <si>
-    <t>_res_.$Step3["step1"]</t>
-  </si>
-  <si>
-    <t>_res_.$Step4["step1"]</t>
-  </si>
-  <si>
-    <t>_res_.$Step5["step1"]</t>
-  </si>
-  <si>
-    <t>_res_.$Step6["step1"]</t>
-  </si>
-  <si>
-    <t>=(Map[][])$Step2["calc"]</t>
-  </si>
-  <si>
-    <t>=(List)$Step2["calc"]</t>
-  </si>
-  <si>
-    <t>=((Map)$Step3[0])["step1"]</t>
-  </si>
-  <si>
-    <t>=((Map)$Step3[1])["step1"]</t>
-  </si>
-  <si>
-    <t>=(Map)((List)(((Map)$Step2[0])["calc"]))[0]</t>
-  </si>
-  <si>
-    <t>=(Map)((List)(((Map)$Step2[0])["calc"]))[1]</t>
-  </si>
-  <si>
-    <t>=(Map)((List)(((Map)$Step2[1])["calc"]))[0]</t>
-  </si>
-  <si>
-    <t>=(Map)((List)(((Map)$Step2[1])["calc"]))[1]</t>
-  </si>
-  <si>
-    <t>=((MyType)(((Map)((List)(((Map)$Step2[1])["calc"]))[1])["step7"])).someMap</t>
-  </si>
-  <si>
-    <t>=(List)$Step1.toMap()["calc"]</t>
-  </si>
-  <si>
-    <t>=$Step2["calc"]</t>
-  </si>
-  <si>
-    <t>=((Passport)((MyType)((Map)$Step4)["step7"]).passportData).passportId</t>
-  </si>
-  <si>
-    <t>=((MyType)((Map)$Step4)["step7"]).someMap</t>
-  </si>
-  <si>
-    <t>=(List)((MyType)((Map)$Step4)["step7"]).someList</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -649,13 +600,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621" rgb="FFFFFF"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485" rgb="9BBB59"/>
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -667,7 +618,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442" rgb="9BBB59"/>
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -764,9 +715,9 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -785,10 +736,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -801,6 +748,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -810,11 +760,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Вычисление" xfId="1" builtinId="22"/>
-    <cellStyle name="Связанная ячейка" xfId="2" builtinId="24"/>
+    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="2" builtinId="24"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -841,7 +792,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -850,17 +801,14 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -898,9 +846,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -933,26 +881,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -985,26 +916,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1177,45 +1091,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="51.59765625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="61.59765625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="24.73046875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="20.3984375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="16.3984375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="21.86328125" collapsed="true"/>
+    <col min="2" max="2" width="21" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="51.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="61.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="29" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="7" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="2" spans="2:8" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B4" s="18" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="E4" s="18" t="s">
+      <c r="C4" s="16"/>
+      <c r="E4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="18"/>
+      <c r="F4" s="16"/>
       <c r="H4" s="8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1232,7 +1146,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1249,7 +1163,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
@@ -1263,7 +1177,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
@@ -1271,7 +1185,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
@@ -1279,7 +1193,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
@@ -1287,7 +1201,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>76</v>
       </c>
@@ -1295,13 +1209,13 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B15" s="16" t="s">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="17"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="C15" s="15"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="11" t="s">
         <v>21</v>
       </c>
@@ -1309,7 +1223,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B17" s="12" t="s">
         <v>32</v>
       </c>
@@ -1317,7 +1231,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B18" s="11" t="s">
         <v>42</v>
       </c>
@@ -1325,7 +1239,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="s">
         <v>78</v>
       </c>
@@ -1333,7 +1247,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B20" s="11" t="s">
         <v>81</v>
       </c>
@@ -1341,7 +1255,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B21" s="11" t="s">
         <v>43</v>
       </c>
@@ -1349,7 +1263,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B22" s="11" t="s">
         <v>44</v>
       </c>
@@ -1357,7 +1271,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:19" ht="45" x14ac:dyDescent="0.25">
       <c r="B23" s="12" t="s">
         <v>39</v>
       </c>
@@ -1365,7 +1279,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:19" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="11" t="s">
         <v>45</v>
       </c>
@@ -1373,7 +1287,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B25" s="12" t="s">
         <v>38</v>
       </c>
@@ -1381,15 +1295,15 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="B28" s="16" t="s">
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B28" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="17"/>
+      <c r="C28" s="15"/>
       <c r="I28" s="2"/>
       <c r="S28" s="2"/>
     </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B29" s="11" t="s">
         <v>21</v>
       </c>
@@ -1397,7 +1311,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B30" s="11" t="s">
         <v>41</v>
       </c>
@@ -1406,34 +1320,34 @@
       </c>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B33" s="14" t="s">
-        <v>160</v>
+    <row r="33" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="22" t="s">
+        <v>178</v>
       </c>
       <c r="C33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="2:9" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B35" s="16" t="s">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="17"/>
+      <c r="C35" s="15"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="11" t="s">
         <v>21</v>
       </c>
@@ -1442,7 +1356,7 @@
       </c>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="11" t="s">
         <v>53</v>
       </c>
@@ -1452,7 +1366,7 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="11" t="s">
         <v>42</v>
       </c>
@@ -1462,7 +1376,7 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="11" t="s">
         <v>58</v>
       </c>
@@ -1472,7 +1386,7 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="11" t="s">
         <v>44</v>
       </c>
@@ -1482,7 +1396,7 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="11" t="s">
         <v>69</v>
       </c>
@@ -1492,7 +1406,7 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="11" t="s">
         <v>45</v>
       </c>
@@ -1502,7 +1416,7 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="11" t="s">
         <v>72</v>
       </c>
@@ -1512,7 +1426,7 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="11" t="s">
         <v>75</v>
       </c>
@@ -1522,7 +1436,7 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="11" t="s">
         <v>83</v>
       </c>
@@ -1532,34 +1446,34 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="11" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>157</v>
+        <v>175</v>
       </c>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I47" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B48" s="16" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B48" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C48" s="19"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="19"/>
-      <c r="G48" s="19"/>
-      <c r="H48" s="19"/>
-      <c r="I48" s="17"/>
-    </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="15"/>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="11" t="s">
         <v>34</v>
       </c>
@@ -1582,10 +1496,10 @@
         <v>89</v>
       </c>
       <c r="I49" s="11" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.45">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="11" t="s">
         <v>34</v>
       </c>
@@ -1608,10 +1522,10 @@
         <v>89</v>
       </c>
       <c r="I50" s="11" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.45">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
         <v>36</v>
       </c>
@@ -1635,13 +1549,13 @@
       </c>
       <c r="I51" s="2"/>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B54" s="15" t="s">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B54" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C54" s="15"/>
-    </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="C54" s="18"/>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="11" t="s">
         <v>21</v>
       </c>
@@ -1649,7 +1563,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="11" t="s">
         <v>40</v>
       </c>
@@ -1657,7 +1571,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="11" t="s">
         <v>46</v>
       </c>
@@ -1665,7 +1579,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="12" t="s">
         <v>63</v>
       </c>
@@ -1673,14 +1587,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B61" s="15" t="s">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B61" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="C61" s="15"/>
+      <c r="C61" s="18"/>
       <c r="H61" s="1"/>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" s="11" t="s">
         <v>21</v>
       </c>
@@ -1688,7 +1602,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" s="11" t="s">
         <v>53</v>
       </c>
@@ -1697,7 +1611,7 @@
       </c>
       <c r="H63" s="1"/>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" s="11" t="s">
         <v>42</v>
       </c>
@@ -1706,46 +1620,46 @@
       </c>
       <c r="H64" s="1"/>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B65" s="11" t="s">
         <v>58</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>181</v>
+        <v>67</v>
       </c>
       <c r="H65" s="1"/>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B66" s="11" t="s">
         <v>44</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.45">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B67" s="11" t="s">
         <v>69</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.45">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C68" s="1"/>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C69" s="1"/>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B71" s="15" t="s">
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B71" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="C71" s="15"/>
-      <c r="D71" s="15"/>
-      <c r="E71" s="15"/>
-    </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="C71" s="18"/>
+      <c r="D71" s="18"/>
+      <c r="E71" s="18"/>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B72" s="11" t="s">
         <v>34</v>
       </c>
@@ -1759,7 +1673,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B73" s="11" t="s">
         <v>34</v>
       </c>
@@ -1773,7 +1687,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B74" s="2">
         <v>1</v>
       </c>
@@ -1787,19 +1701,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B76" s="14" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="77" spans="2:8" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B78" s="15" t="s">
+    <row r="76" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="22" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B78" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="C78" s="15"/>
-    </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="C78" s="18"/>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B79" s="11" t="s">
         <v>21</v>
       </c>
@@ -1807,7 +1721,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B80" s="12" t="s">
         <v>102</v>
       </c>
@@ -1815,7 +1729,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B81" s="12" t="s">
         <v>103</v>
       </c>
@@ -1823,7 +1737,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B82" s="12" t="s">
         <v>104</v>
       </c>
@@ -1831,7 +1745,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B83" s="12" t="s">
         <v>105</v>
       </c>
@@ -1839,7 +1753,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B84" s="12" t="s">
         <v>106</v>
       </c>
@@ -1847,7 +1761,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B85" s="12" t="s">
         <v>63</v>
       </c>
@@ -1855,14 +1769,14 @@
         <v>52</v>
       </c>
     </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B89" s="15" t="s">
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B89" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C89" s="15"/>
+      <c r="C89" s="18"/>
       <c r="G89" s="1"/>
     </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B90" s="11" t="s">
         <v>21</v>
       </c>
@@ -1870,7 +1784,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B91" s="11" t="s">
         <v>53</v>
       </c>
@@ -1879,7 +1793,7 @@
       </c>
       <c r="G91" s="1"/>
     </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B92" s="11" t="s">
         <v>42</v>
       </c>
@@ -1888,16 +1802,16 @@
       </c>
       <c r="G92" s="1"/>
     </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B93" s="11" t="s">
         <v>58</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>190</v>
+        <v>107</v>
       </c>
       <c r="G93" s="1"/>
     </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B94" s="11" t="s">
         <v>44</v>
       </c>
@@ -1905,40 +1819,40 @@
         <v>109</v>
       </c>
     </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B95" s="11" t="s">
         <v>45</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.45">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B96" s="11" t="s">
         <v>75</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.45">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B97" s="11" t="s">
         <v>83</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B101" s="15" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B101" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="C101" s="15"/>
-      <c r="D101" s="15"/>
-      <c r="E101" s="15"/>
-      <c r="F101" s="15"/>
-    </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="C101" s="18"/>
+      <c r="D101" s="18"/>
+      <c r="E101" s="18"/>
+      <c r="F101" s="18"/>
+    </row>
+    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B102" s="11" t="s">
         <v>34</v>
       </c>
@@ -1955,7 +1869,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B103" s="11" t="s">
         <v>34</v>
       </c>
@@ -1972,7 +1886,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B104" s="2">
         <v>1</v>
       </c>
@@ -1991,59 +1905,59 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B101:F101"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B71:E71"/>
+    <mergeCell ref="B61:C61"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B35:C35"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="B48:I48"/>
     <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B101:F101"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B71:E71"/>
-    <mergeCell ref="B61:C61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M85"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="22.1328125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="52.3984375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="29.59765625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="27.3984375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="33.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="28.1328125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="13.59765625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="12.86328125" collapsed="true"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="52.42578125" customWidth="1"/>
+    <col min="4" max="4" width="29.5703125" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" customWidth="1"/>
+    <col min="7" max="7" width="33" customWidth="1"/>
+    <col min="8" max="8" width="28.140625" customWidth="1"/>
+    <col min="9" max="9" width="29" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="5" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
       <c r="C1" s="6"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="B3" s="21" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="C3" s="22"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="C3" s="21"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" s="11" t="s">
         <v>21</v>
       </c>
@@ -2051,7 +1965,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
         <v>40</v>
       </c>
@@ -2059,7 +1973,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
         <v>46</v>
       </c>
@@ -2067,7 +1981,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
         <v>99</v>
       </c>
@@ -2075,17 +1989,17 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="B9" s="20" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="C9" s="20"/>
+      <c r="C9" s="19"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
         <v>21</v>
       </c>
@@ -2093,7 +2007,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" s="11" t="s">
         <v>53</v>
       </c>
@@ -2102,7 +2016,7 @@
       </c>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" s="11" t="s">
         <v>42</v>
       </c>
@@ -2111,16 +2025,16 @@
       </c>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
         <v>58</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>180</v>
+        <v>114</v>
       </c>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
         <v>44</v>
       </c>
@@ -2129,7 +2043,7 @@
       </c>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" s="11" t="s">
         <v>69</v>
       </c>
@@ -2138,7 +2052,7 @@
       </c>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16" s="11" t="s">
         <v>45</v>
       </c>
@@ -2147,7 +2061,7 @@
       </c>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="11" t="s">
         <v>72</v>
       </c>
@@ -2156,64 +2070,64 @@
       </c>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="11" t="s">
         <v>75</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.45">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="s">
         <v>83</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.45">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="11" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="11" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.45">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B25" s="20" t="s">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B25" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="20"/>
-      <c r="M25" s="20"/>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="11" t="s">
         <v>120</v>
       </c>
@@ -2227,31 +2141,31 @@
         <v>123</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>162</v>
+        <v>131</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>163</v>
+        <v>132</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>164</v>
+        <v>133</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>165</v>
+        <v>134</v>
       </c>
       <c r="J26" s="11" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="K26" s="11" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="L26" s="11" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="M26" s="11" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.45">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="11" t="s">
         <v>120</v>
       </c>
@@ -2265,31 +2179,31 @@
         <v>123</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>162</v>
+        <v>131</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>163</v>
+        <v>132</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>164</v>
+        <v>133</v>
       </c>
       <c r="I27" s="11" t="s">
-        <v>165</v>
+        <v>134</v>
       </c>
       <c r="J27" s="11" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="K27" s="11" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="L27" s="11" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="M27" s="11" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.45">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
         <v>1</v>
       </c>
@@ -2327,22 +2241,22 @@
         <v>125</v>
       </c>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B32" s="20" t="s">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B32" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="C32" s="20"/>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="C32" s="19"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="11" t="s">
         <v>21</v>
       </c>
@@ -2350,7 +2264,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="11" t="s">
         <v>40</v>
       </c>
@@ -2358,7 +2272,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="11" t="s">
         <v>46</v>
       </c>
@@ -2366,7 +2280,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" s="12" t="s">
         <v>99</v>
       </c>
@@ -2374,18 +2288,18 @@
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B41" s="20" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="C41" s="20"/>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="C41" s="19"/>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" s="11" t="s">
         <v>21</v>
       </c>
@@ -2393,7 +2307,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" s="11" t="s">
         <v>53</v>
       </c>
@@ -2401,7 +2315,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" s="11" t="s">
         <v>42</v>
       </c>
@@ -2409,101 +2323,101 @@
         <v>64</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" s="11" t="s">
         <v>58</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.45">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" s="11" t="s">
         <v>44</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.45">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" s="11" t="s">
         <v>69</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.45">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" s="11" t="s">
         <v>45</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.45">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B49" s="11" t="s">
         <v>72</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.45">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B50" s="11" t="s">
         <v>75</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.45">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B51" s="11" t="s">
         <v>83</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.45">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B52" s="11" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.45">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B53" s="11" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.45">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C54" s="1"/>
     </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C55" s="1"/>
     </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B57" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="C57" s="20"/>
-      <c r="D57" s="20"/>
-      <c r="E57" s="20"/>
-      <c r="F57" s="20"/>
-      <c r="G57" s="20"/>
-      <c r="H57" s="20"/>
-      <c r="I57" s="20"/>
-      <c r="J57" s="20"/>
-      <c r="K57" s="20"/>
-      <c r="L57" s="20"/>
-      <c r="M57" s="20"/>
-    </row>
-    <row r="58" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B57" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="C57" s="19"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="19"/>
+      <c r="G57" s="19"/>
+      <c r="H57" s="19"/>
+      <c r="I57" s="19"/>
+      <c r="J57" s="19"/>
+      <c r="K57" s="19"/>
+      <c r="L57" s="19"/>
+      <c r="M57" s="19"/>
+    </row>
+    <row r="58" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B58" s="11" t="s">
         <v>120</v>
       </c>
@@ -2517,31 +2431,31 @@
         <v>123</v>
       </c>
       <c r="F58" s="11" t="s">
-        <v>162</v>
+        <v>131</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>163</v>
+        <v>132</v>
       </c>
       <c r="H58" s="11" t="s">
-        <v>164</v>
+        <v>133</v>
       </c>
       <c r="I58" s="11" t="s">
-        <v>165</v>
+        <v>134</v>
       </c>
       <c r="J58" s="11" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="K58" s="11" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="L58" s="11" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="M58" s="11" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="59" spans="2:13" x14ac:dyDescent="0.45">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="59" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B59" s="11" t="s">
         <v>120</v>
       </c>
@@ -2555,31 +2469,31 @@
         <v>123</v>
       </c>
       <c r="F59" s="11" t="s">
-        <v>162</v>
+        <v>131</v>
       </c>
       <c r="G59" s="11" t="s">
-        <v>163</v>
+        <v>132</v>
       </c>
       <c r="H59" s="11" t="s">
-        <v>164</v>
+        <v>133</v>
       </c>
       <c r="I59" s="11" t="s">
-        <v>165</v>
+        <v>134</v>
       </c>
       <c r="J59" s="11" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="K59" s="11" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="L59" s="11" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="M59" s="11" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="60" spans="2:13" x14ac:dyDescent="0.45">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="60" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B60" s="2">
         <v>1</v>
       </c>
@@ -2617,19 +2531,19 @@
         <v>125</v>
       </c>
     </row>
-    <row r="63" spans="2:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="63" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="64" spans="2:13" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B66" s="20" t="s">
-        <v>145</v>
-      </c>
-      <c r="C66" s="20"/>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.45">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="64" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="C66" s="19"/>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" s="11" t="s">
         <v>21</v>
       </c>
@@ -2637,23 +2551,23 @@
         <v>33</v>
       </c>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" s="11" t="s">
         <v>40</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.45">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" s="11" t="s">
         <v>46</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.45">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" s="11" t="s">
         <v>99</v>
       </c>
@@ -2662,13 +2576,13 @@
       </c>
       <c r="D70" s="1"/>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B72" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="C72" s="20"/>
-    </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B72" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="C72" s="19"/>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" s="11" t="s">
         <v>21</v>
       </c>
@@ -2676,120 +2590,120 @@
         <v>22</v>
       </c>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" s="11" t="s">
         <v>53</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.45">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75" s="11" t="s">
         <v>42</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.45">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B76" s="11" t="s">
         <v>58</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.45">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" s="11" t="s">
         <v>44</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.45">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" s="11" t="s">
         <v>69</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.45">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" s="11" t="s">
         <v>45</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" s="11" t="s">
         <v>72</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B82" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="C82" s="20"/>
-      <c r="D82" s="20"/>
-      <c r="E82" s="20"/>
-      <c r="F82" s="20"/>
-      <c r="G82" s="20"/>
-      <c r="H82" s="20"/>
-    </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.45">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B82" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="C82" s="19"/>
+      <c r="D82" s="19"/>
+      <c r="E82" s="19"/>
+      <c r="F82" s="19"/>
+      <c r="G82" s="19"/>
+      <c r="H82" s="19"/>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B83" s="11" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="C83" s="11" t="s">
         <v>35</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E83" s="11" t="s">
-        <v>162</v>
+        <v>131</v>
       </c>
       <c r="F83" s="11" t="s">
-        <v>163</v>
+        <v>132</v>
       </c>
       <c r="G83" s="11" t="s">
-        <v>164</v>
+        <v>133</v>
       </c>
       <c r="H83" s="11" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.45">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B84" s="11" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="C84" s="11" t="s">
         <v>35</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="E84" s="11" t="s">
-        <v>177</v>
+        <v>130</v>
       </c>
       <c r="F84" s="11" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="G84" s="11" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="H84" s="11" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.45">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B85" s="2">
         <v>1</v>
       </c>
@@ -2829,12 +2743,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>